<commit_message>
quase todos os anexos
</commit_message>
<xml_diff>
--- a/filtros.xlsx
+++ b/filtros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.ferrari\Documents\R\automate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3561AB-01D9-4140-B863-088CF98E707E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714F830D-1C7A-43C8-A626-5D2B4477069A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{35A31CFB-0D6A-4E5D-AD17-F59A1D4E70CF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{35A31CFB-0D6A-4E5D-AD17-F59A1D4E70CF}"/>
   </bookViews>
   <sheets>
     <sheet name="filtros_linhas" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="514">
   <si>
     <t>demonstrativo</t>
   </si>
@@ -1584,6 +1584,15 @@
   </si>
   <si>
     <t>Natureza Despesa Detalhada Código</t>
+  </si>
+  <si>
+    <t>fonte_recursos_detalhada_codigo</t>
+  </si>
+  <si>
+    <t>Fonte de Recurso Detalhada</t>
+  </si>
+  <si>
+    <t>plano_orcamentario_codigo_po</t>
   </si>
 </sst>
 </file>
@@ -10573,7 +10582,7 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11470,7 +11479,7 @@
         <v>446</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>484</v>
+        <v>513</v>
       </c>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
@@ -12997,8 +13006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D527EEA-838C-472C-B303-51890342D295}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13122,41 +13131,41 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="12" t="s">
-        <v>414</v>
+        <v>433</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>459</v>
+        <v>476</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>186</v>
+        <v>63</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>457</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="12" t="s">
-        <v>414</v>
+        <v>433</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>459</v>
+        <v>476</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>186</v>
+        <v>63</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="12" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>493</v>
+        <v>186</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>457</v>
@@ -13164,16 +13173,16 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="12" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>493</v>
+        <v>186</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>457</v>
+        <v>415</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -13201,7 +13210,7 @@
         <v>493</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>415</v>
+        <v>457</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -13215,7 +13224,7 @@
         <v>493</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>418</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -13229,35 +13238,35 @@
         <v>493</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="12" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>459</v>
+        <v>476</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>192</v>
+        <v>493</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>457</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="12" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>459</v>
+        <v>476</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>192</v>
+        <v>493</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>409</v>
+        <v>417</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -13271,7 +13280,7 @@
         <v>192</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>410</v>
+        <v>457</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -13285,7 +13294,7 @@
         <v>192</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -13299,77 +13308,77 @@
         <v>192</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>494</v>
+        <v>192</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>492</v>
+        <v>459</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>492</v>
+        <v>476</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>172</v>
+        <v>494</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="12" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>492</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>457</v>
+        <v>409</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="12" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>492</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>408</v>
+        <v>422</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -13383,7 +13392,7 @@
         <v>200</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>410</v>
+        <v>457</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -13397,7 +13406,7 @@
         <v>200</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -13411,7 +13420,7 @@
         <v>200</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -13425,7 +13434,7 @@
         <v>200</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -13439,88 +13448,88 @@
         <v>200</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="12" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>492</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>495</v>
+        <v>200</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="12" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>492</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>496</v>
+        <v>200</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="12" t="s">
-        <v>429</v>
+        <v>512</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>459</v>
+        <v>137</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>178</v>
+        <v>511</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>458</v>
+        <v>428</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="12" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>459</v>
+        <v>492</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>178</v>
+        <v>511</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>409</v>
+        <v>425</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>459</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>459</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>409</v>
@@ -13537,7 +13546,7 @@
         <v>188</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>415</v>
+        <v>457</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -13551,7 +13560,7 @@
         <v>188</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -13565,7 +13574,7 @@
         <v>188</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -13579,49 +13588,49 @@
         <v>188</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>459</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B43" s="12" t="s">
         <v>459</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>459</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -13635,35 +13644,35 @@
         <v>196</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>63</v>
+        <v>196</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>63</v>
+        <v>196</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -13752,16 +13761,16 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="12" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>137</v>
+        <v>459</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>208</v>
+        <v>509</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>457</v>
+        <v>415</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -13775,7 +13784,7 @@
         <v>208</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>408</v>
+        <v>457</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -13789,7 +13798,7 @@
         <v>208</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -13803,7 +13812,7 @@
         <v>208</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -13817,7 +13826,7 @@
         <v>208</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -13831,21 +13840,21 @@
         <v>208</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>459</v>
+        <v>137</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>509</v>
+        <v>208</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>415</v>
+        <v>428</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -14116,30 +14125,30 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="12" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="B80" s="12" t="s">
         <v>459</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>484</v>
+        <v>502</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="12" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B81" s="12" t="s">
         <v>459</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>182</v>
+        <v>513</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -14153,35 +14162,35 @@
         <v>182</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>492</v>
+        <v>459</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>501</v>
+        <v>182</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>443</v>
+        <v>413</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>459</v>
+        <v>492</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>180</v>
+        <v>501</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -14209,7 +14218,7 @@
         <v>180</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -14223,7 +14232,7 @@
         <v>180</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>410</v>
+        <v>458</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -14237,12 +14246,12 @@
         <v>180</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B89" s="12" t="s">
         <v>459</v>
@@ -14251,21 +14260,21 @@
         <v>180</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B90" s="12" t="s">
         <v>459</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>502</v>
+        <v>180</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -14284,7 +14293,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="12" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B92" s="12" t="s">
         <v>492</v>
@@ -14293,7 +14302,7 @@
         <v>176</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>415</v>
+        <v>457</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -14307,12 +14316,12 @@
         <v>176</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>457</v>
+        <v>409</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="12" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B94" s="12" t="s">
         <v>492</v>
@@ -14321,7 +14330,7 @@
         <v>176</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -14340,39 +14349,40 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="12" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B96" s="12" t="s">
         <v>492</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>413</v>
+        <v>425</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="12" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B97" s="12" t="s">
         <v>492</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>490</v>
+        <v>504</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D97" xr:uid="{3D527EEA-838C-472C-B303-51890342D295}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D97">
-      <sortCondition ref="A1:A97"/>
+      <sortCondition ref="C1:C97"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -14380,7 +14390,7 @@
           <x14:formula1>
             <xm:f>atributos!$B$2:$B$100</xm:f>
           </x14:formula1>
-          <xm:sqref>C97:C98 C2:C95</xm:sqref>
+          <xm:sqref>C97:C98 C2:C94</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14389,6 +14399,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007CAF85F579D9C94D829ACD7F874C94AF" ma:contentTypeVersion="17" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="131b27aa05929388ee065934bbaf2bd9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0f370953-9f60-49f5-9e00-e1a3f0ed2ba0" xmlns:ns3="a77d5170-f388-44e7-ac79-04d186fae979" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f2e4360ae98a7aac94ddb8c7d52d155" ns2:_="" ns3:_="">
     <xsd:import namespace="0f370953-9f60-49f5-9e00-e1a3f0ed2ba0"/>
@@ -14631,15 +14650,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -14653,6 +14663,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14994FB0-1245-4FF0-9647-9FCB93A1C938}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C206B9F-1746-4368-8EC2-BEED99B13E82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14667,14 +14685,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14994FB0-1245-4FF0-9647-9FCB93A1C938}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>